<commit_message>
record button& button entry update
when not click ,record button show status and capacity, and when clicked, show record.
button entry only use to start timing or counting
________________________finished above________________________________

___________________unfinished below ________________________________
add manual input button to record panel, and when click, open inputpanel
show infinity scrollview at record panel
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -296,6 +296,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -603,7 +604,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,6 +730,9 @@
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C14" s="15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="1" t="s">
@@ -747,11 +751,6 @@
     <row r="17" spans="1:2">
       <c r="B17" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="B18" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2">

</xml_diff>

<commit_message>
counter total newday  initialization update
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -604,7 +604,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -714,7 +714,7 @@
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -722,7 +722,7 @@
       <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="15" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add icon into main.scene
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -365,7 +365,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,9 +397,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,6 +432,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -606,11 +608,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,7 +708,7 @@
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C11" t="s">
@@ -728,7 +730,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="15" t="s">
@@ -739,7 +741,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -837,7 +839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Record Panel auto size adjustment
1.manual input button color fixed
2.records panel size auto adjust by text
3. show total amout at last before next dayline
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>record+滾屏  顯示只截取最近7天</t>
+  </si>
+  <si>
+    <t>record panel根據文字調整大小，增加前日總量</t>
   </si>
 </sst>
 </file>
@@ -603,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -752,6 +755,11 @@
       </c>
       <c r="D15" s="12">
         <v>43179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3">

</xml_diff>

<commit_message>
title today amount/duration reset
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,7 +929,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="7" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "title today amount/duration reset""
This reverts commit c108e3cd2dd107418870770e338713132506b053, reversing
changes made to 8e3ae0eabfd72459358202764917299844b1d1f1.
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,7 +929,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="7" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
today duration debug after record deleted
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -263,16 +264,37 @@
     <t>refresh nappy amount</t>
   </si>
   <si>
-    <t>adjust record panel layout</t>
-  </si>
-  <si>
     <t>button entry and panel input code optimizing</t>
+  </si>
+  <si>
+    <t>main，calendar icon</t>
+  </si>
+  <si>
+    <t>record panel scrollbar hide</t>
+  </si>
+  <si>
+    <t>adjust record panel layout,load more text size</t>
+  </si>
+  <si>
+    <t>debug calendar log type chose panel 按退出鍵時未回到calendar</t>
+  </si>
+  <si>
+    <t>debug calendar note editor界面按退出鍵未退出</t>
+  </si>
+  <si>
+    <t>calendar note editor input holder text size adjust</t>
+  </si>
+  <si>
+    <t>change total @main record after record deleted（timer&amp;counter）</t>
+  </si>
+  <si>
+    <t>change total @main record after record deleted（nappy）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -361,7 +383,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -395,6 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -457,7 +480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,10 +512,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -524,7 +546,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -700,11 +721,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -994,7 +1027,7 @@
         <v>43219</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>78</v>
@@ -1002,83 +1035,107 @@
     </row>
     <row r="35" spans="1:3">
       <c r="B35" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="B36"/>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="B37"/>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38"/>
+      <c r="C38" s="15" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39"/>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40"/>
+      <c r="C40" s="15" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2" t="s">
+      <c r="C41" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="C42" s="21"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B52" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="2" t="s">
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="B47" s="1" t="s">
+    <row r="58" spans="1:2">
+      <c r="B58" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="B48" s="1" t="s">
+    <row r="59" spans="1:2">
+      <c r="B59" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="1" t="s">
+    <row r="61" spans="1:2">
+      <c r="B61" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="1" t="s">
+    <row r="62" spans="1:2">
+      <c r="B62" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="1" t="s">
+    <row r="63" spans="1:2">
+      <c r="B63" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="1" t="s">
+    <row r="64" spans="1:2">
+      <c r="B64" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="1" t="s">
+    <row r="65" spans="2:2">
+      <c r="B65" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
-      <c r="B56" t="s">
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1088,8 +1145,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
baby info scene -- baby age show in different unit
age show in days / day&week / week&month / month&year
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -255,9 +255,6 @@
     <t>打開app為新一日時，即使無新record加入也能顯示日期分割綫和之前一日total amount</t>
   </si>
   <si>
-    <t>baby info的age 改爲button，切換顯示天，月，年</t>
-  </si>
-  <si>
     <t>refresh today amount after a record is deleted</t>
   </si>
   <si>
@@ -289,6 +286,12 @@
   </si>
   <si>
     <t>change total @main record after record deleted（nappy）</t>
+  </si>
+  <si>
+    <t>baby info的age 改爲button，切換顯示天，天周，周月，月年</t>
+  </si>
+  <si>
+    <t>calendar增加growth log</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -417,7 +420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -737,7 +739,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,7 +1007,7 @@
         <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>76</v>
@@ -1016,7 +1018,7 @@
         <v>43213</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>77</v>
@@ -1027,7 +1029,7 @@
         <v>43219</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>78</v>
@@ -1035,44 +1037,44 @@
     </row>
     <row r="35" spans="1:3">
       <c r="B35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38"/>
       <c r="C38" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39"/>
       <c r="C39" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="B40"/>
       <c r="C40" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1081,7 +1083,9 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="C42" s="21"/>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">

</xml_diff>

<commit_message>
calendar  next/previous year  button
1. calendar 選擇不同年份
2. 百日和整嵗生日紅色bold顯示
2 plan update
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -225,9 +225,6 @@
     <t>calendar插入圖片，並可查看所有照片</t>
   </si>
   <si>
-    <t>Select date on calendar</t>
-  </si>
-  <si>
     <t>calendar插入不同模式note，text note，reminder，growth，圖片</t>
   </si>
   <si>
@@ -309,10 +306,13 @@
     <t>title total amout 每日自動清零後 reset title</t>
   </si>
   <si>
-    <t>calendar增加百日提醒</t>
-  </si>
-  <si>
     <t>增加正在計時的當日記錄</t>
+  </si>
+  <si>
+    <t>calendar增加百日提醒，生日和百日用紅色bold顯示</t>
+  </si>
+  <si>
+    <t>Select date on calendar，year ++</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -439,7 +439,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -760,7 +759,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -934,7 +933,7 @@
       <c r="A19" s="12">
         <v>43186</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -974,7 +973,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -983,7 +982,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -991,15 +990,15 @@
         <v>61</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>74</v>
+      <c r="C26" s="19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1025,13 +1024,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1039,10 +1038,10 @@
         <v>43213</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1050,81 +1049,81 @@
         <v>43219</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="C37" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="B41"/>
       <c r="C41" s="19" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42"/>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="C43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="C44" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="C45" t="s">
+      <c r="C45" s="15" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1138,7 +1137,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="B53" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1176,7 +1175,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="B64" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="2:2">
@@ -1191,7 +1190,7 @@
     </row>
     <row r="67" spans="2:2">
       <c r="B67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plan update & debug
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>Select date on calendar，year ++</t>
+  </si>
+  <si>
+    <t>標尺icon顯示在calendar add log的增加growth記錄前面</t>
   </si>
 </sst>
 </file>
@@ -759,7 +762,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1156,6 +1159,11 @@
     <row r="59" spans="1:2">
       <c r="B59" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="B60" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:2">

</xml_diff>

<commit_message>
baby info growth button optimized
1. delete button_input prefab and cs file
2. growth add button using a same inputfield
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -316,12 +316,15 @@
   </si>
   <si>
     <t>標尺icon顯示在calendar add log的增加growth記錄前面</t>
+  </si>
+  <si>
+    <t>baby info growth button優化，共用一個inputfield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -505,7 +508,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,10 +540,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,7 +574,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -748,7 +749,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -760,11 +761,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1132,6 +1133,11 @@
         <v>97</v>
       </c>
     </row>
+    <row r="46" spans="1:3">
+      <c r="C46" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
         <v>7</v>
@@ -1210,7 +1216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
manual input an ongoing timing record
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -319,12 +319,18 @@
   </si>
   <si>
     <t>baby info growth button優化，共用一個inputfield</t>
+  </si>
+  <si>
+    <t>manual input an ongoing timing record</t>
+  </si>
+  <si>
+    <t>finish an ongoing timing record before delete it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -508,7 +514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -540,9 +546,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,6 +581,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -749,7 +757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -761,11 +769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1078,13 +1086,16 @@
       </c>
     </row>
     <row r="37" spans="1:3">
+      <c r="B37" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="C37" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>82</v>
@@ -1092,7 +1103,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="B39" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>83</v>
@@ -1100,20 +1111,21 @@
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="15" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="B41"/>
+      <c r="B41" s="15" t="s">
+        <v>102</v>
+      </c>
       <c r="C41" s="19" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="B42"/>
       <c r="C42" t="s">
         <v>88</v>
       </c>
@@ -1216,7 +1228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
log text size adjust
1. adjust the size of the log in calendar
2. plan update
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>debug 點擊非本月日期添加log時，顯示logeditor界面失敗</t>
+  </si>
+  <si>
+    <t>week 9</t>
+  </si>
+  <si>
+    <t>debug 退出或切換界面時log無法保存</t>
+  </si>
+  <si>
+    <t>增加了calendar logadd裏weight 和height的icon</t>
+  </si>
+  <si>
+    <t>同步calendar的growth add 和 baby info界面的growth記錄</t>
   </si>
 </sst>
 </file>
@@ -764,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B12:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12:B30"/>
     </sheetView>
   </sheetViews>
@@ -873,10 +885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1263,74 +1275,97 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="2" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="12">
+        <v>43224</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="12"/>
+      <c r="C51" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="B53" s="1" t="s">
+    <row r="54" spans="1:3">
+      <c r="B54" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="B58" s="1" t="s">
+    <row r="59" spans="1:3">
+      <c r="B59" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="B59" s="1" t="s">
+    <row r="60" spans="1:3">
+      <c r="B60" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:3">
+      <c r="B61" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:3">
+      <c r="B62" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="B62" s="1" t="s">
+    <row r="63" spans="1:3">
+      <c r="B63" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="1:3">
+      <c r="B64" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="B64" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add reset baby info
1. add reset baby info
2. add new icon for setting in scene baby info panel
3. update plan and add user feedbacks
4. add function: press Key Escape in babyInfo/ pattern/ calendar to quit application
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="測試情況" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -343,6 +344,36 @@
   </si>
   <si>
     <t>同步calendar的growth add 和 baby info界面的growth記錄</t>
+  </si>
+  <si>
+    <t>手機品牌</t>
+  </si>
+  <si>
+    <t>手機型號</t>
+  </si>
+  <si>
+    <t>安卓版本</t>
+  </si>
+  <si>
+    <t>測試情況</t>
+  </si>
+  <si>
+    <t>小米</t>
+  </si>
+  <si>
+    <t>MI 5S</t>
+  </si>
+  <si>
+    <t>6.0.1</t>
+  </si>
+  <si>
+    <t>可用</t>
+  </si>
+  <si>
+    <t>修改意見</t>
+  </si>
+  <si>
+    <t>返回鍵退出整個程序</t>
   </si>
 </sst>
 </file>
@@ -887,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -1446,4 +1477,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
week 10 plan update & debug
1.entry 左側圖標點擊可以開啓計時/計次
2.debug 在更改growth存儲方式后不能更新daily estimate
3. week 10 plan update
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="測試情況" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Add customise button in main menu</t>
   </si>
   <si>
-    <t>Record scene, show all types of records in the same scene/ show chart</t>
-  </si>
-  <si>
     <t>功能框架</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>record panel根據文字調整大小，增加前日總量</t>
   </si>
   <si>
-    <t>setting the layout to fit different resolutions</t>
-  </si>
-  <si>
     <t>week 5</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>Select date on calendar，year ++</t>
   </si>
   <si>
-    <t>標尺icon顯示在calendar add log的增加growth記錄前面</t>
-  </si>
-  <si>
     <t>baby info growth button優化，共用一個inputfield</t>
   </si>
   <si>
@@ -374,6 +365,45 @@
   </si>
   <si>
     <t>返回鍵退出整個程序</t>
+  </si>
+  <si>
+    <t>week 10</t>
+  </si>
+  <si>
+    <t>debug 更改growth存儲模式后daily estimate 不能顯示</t>
+  </si>
+  <si>
+    <t>分辨率自適應</t>
+  </si>
+  <si>
+    <t>增加輔食模塊，記錄吃的時間和食物類型，不用記錄吃的量，可使用input 為text的counter</t>
+  </si>
+  <si>
+    <t>刪除記錄後title顯示不正常，title仍為未刪除記錄前的狀態</t>
+  </si>
+  <si>
+    <t>setting icon</t>
+  </si>
+  <si>
+    <t>baby info增加reset baby info功能</t>
+  </si>
+  <si>
+    <t>增加了keyboard按鈕退出app</t>
+  </si>
+  <si>
+    <t>calendar 增加growth添加了標尺和刻度盤icon</t>
+  </si>
+  <si>
+    <t>growth icon：height &amp; weight</t>
+  </si>
+  <si>
+    <t>找個好看的字體</t>
+  </si>
+  <si>
+    <t>calendar界面查看所有logs或分類查看logs</t>
+  </si>
+  <si>
+    <t>entry左側圖標也可點擊計時/計次</t>
   </si>
 </sst>
 </file>
@@ -468,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -501,6 +531,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -805,6 +838,547 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1">
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="12">
+        <v>43174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="12">
+        <v>43177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="12">
+        <v>43175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="12">
+        <v>43178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="12">
+        <v>43179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="12">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="12">
+        <v>43186</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="12">
+        <v>43188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" s="18" customFormat="1">
+      <c r="A22" s="17">
+        <v>43196</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="12">
+        <v>43212</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="12"/>
+      <c r="B24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="12">
+        <v>43213</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="12">
+        <v>43219</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="B36" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="C42" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="C44" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="C45" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="C46" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="C47" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="C48" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="12">
+        <v>43224</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="12">
+        <v>43227</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="12"/>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="12"/>
+      <c r="C53" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="20"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="12">
+        <v>43236</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="12">
+        <v>43242</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="C60" s="13"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="B67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="B68" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="B69" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="B71" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="B72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B12:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -911,498 +1485,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D68"/>
-  <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="12">
-        <v>43174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="12">
-        <v>43177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="12">
-        <v>43175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="12">
-        <v>43178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="12">
-        <v>43179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="B16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="12">
-        <v>43181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="12">
-        <v>43186</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="12">
-        <v>43188</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" s="18" customFormat="1">
-      <c r="A22" s="17">
-        <v>43196</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="12">
-        <v>43212</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="12"/>
-      <c r="B24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="B25" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="B26" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="B27" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="B28" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="B29" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="B30"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="B31"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="12">
-        <v>43213</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="12">
-        <v>43219</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="B35" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="B36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="B37" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="B38" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="B39" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="B40" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="B41" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="C42" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="C43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="C44" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="C45" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="C46" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="C47" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="C48" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="12">
-        <v>43224</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="12"/>
-      <c r="C51" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="B54" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="B59" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="B60" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="B61" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="B63" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="B64" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1422,56 +1504,56 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1483,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1498,36 +1580,36 @@
   <sheetData>
     <row r="1" spans="2:6">
       <c r="B1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>112</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
         <v>113</v>
       </c>
-      <c r="C2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add solid food button v0.5
1.add solid food button
2. need to fix solid food record and manual input entry solid food
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -388,9 +388,6 @@
     <t>baby info增加reset baby info功能</t>
   </si>
   <si>
-    <t>增加了keyboard按鈕退出app</t>
-  </si>
-  <si>
     <t>calendar 增加growth添加了標尺和刻度盤icon</t>
   </si>
   <si>
@@ -404,6 +401,12 @@
   </si>
   <si>
     <t>entry左側圖標也可點擊計時/計次</t>
+  </si>
+  <si>
+    <t>back key quit application(main)</t>
+  </si>
+  <si>
+    <t>增加了keyboard按鈕退出app(calendar / pattern / baby info)</t>
   </si>
 </sst>
 </file>
@@ -841,7 +844,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1255,7 +1258,7 @@
         <v>43227</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>105</v>
@@ -1273,14 +1276,14 @@
     <row r="53" spans="1:3">
       <c r="A53" s="12"/>
       <c r="C53" s="15" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="20"/>
       <c r="B54" s="21"/>
       <c r="C54" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1313,14 +1316,19 @@
         <v>120</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="C59" s="15" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debugs & plan update
1. debug ： calendar改變age顯示方式時離整月不到一周時會顯示整月
2. debug ：calendar無記錄時title顯示為1 jan 1
3. 增加main界面 按鍵盤回退鍵 退出程序
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>增加了keyboard按鈕退出app(calendar / pattern / baby info)</t>
+  </si>
+  <si>
+    <t>debug calendar無記錄時title顯示為1 jan 1</t>
+  </si>
+  <si>
+    <t>debug： calendar改變age顯示方式時離整月不到一周時會顯示整月</t>
   </si>
 </sst>
 </file>
@@ -841,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1301,10 +1307,7 @@
       <c r="A56" s="12">
         <v>43236</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="C56" s="15" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1315,7 +1318,7 @@
       <c r="B57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="7" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1333,49 +1336,61 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="C60" s="13"/>
+      <c r="C60" s="7" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2" t="s">
+      <c r="C61" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="C62" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="2" t="s">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="B67" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="B68" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="B69" s="1" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="B70" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="B72" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="B73" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="B72" t="s">
+    <row r="74" spans="1:2">
+      <c r="B74" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Icon+1 & nappy record total debug
</commit_message>
<xml_diff>
--- a/plan/optimization plan.xlsx
+++ b/plan/optimization plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="測試情況" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
   <si>
     <t>Baby photo input</t>
   </si>
@@ -416,12 +416,18 @@
   </si>
   <si>
     <t>遠程同步記錄，可做成付費版功能</t>
+  </si>
+  <si>
+    <t>Nappy record total debug</t>
+  </si>
+  <si>
+    <t>Solid Food Icon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -510,7 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -546,6 +552,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -608,7 +615,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,9 +647,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,6 +682,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -849,11 +858,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1299,7 +1308,7 @@
       <c r="A55" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C55" s="15" t="s">
@@ -1310,6 +1319,9 @@
       <c r="A56" s="12">
         <v>43236</v>
       </c>
+      <c r="B56" s="19" t="s">
+        <v>133</v>
+      </c>
       <c r="C56" s="15" t="s">
         <v>118</v>
       </c>
@@ -1318,7 +1330,7 @@
       <c r="A57" s="12">
         <v>43242</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="7" t="s">
         <v>120</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -1334,6 +1346,9 @@
       </c>
     </row>
     <row r="59" spans="1:3">
+      <c r="B59" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="C59" s="15" t="s">
         <v>128</v>
       </c>
@@ -1409,7 +1424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B12:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1520,7 +1535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1593,7 +1608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>